<commit_message>
Support numeric and fomula cells #18
(cherry picked from commit 6a9e696035b3b626de7069825f0ab84d5362d51d)
</commit_message>
<xml_diff>
--- a/sample/report/template/sheet_02.xlsx
+++ b/sample/report/template/sheet_02.xlsx
@@ -226,7 +226,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -237,6 +237,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1378,9 +1381,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="D1" s="4">
+        <v>123</v>
+      </c>
+      <c r="E1" s="4">
+        <v>456</v>
+      </c>
+      <c r="F1" s="4">
+        <f>D1+E1</f>
+        <v>579</v>
+      </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -1388,13 +1398,13 @@
     </row>
     <row r="2" ht="15" customHeight="1">
       <c r="A2" s="2"/>
-      <c r="B2" t="s" s="4">
+      <c r="B2" t="s" s="5">
         <v>1</v>
       </c>
-      <c r="C2" t="s" s="4">
+      <c r="C2" t="s" s="5">
         <v>2</v>
       </c>
-      <c r="D2" t="s" s="4">
+      <c r="D2" t="s" s="5">
         <v>3</v>
       </c>
       <c r="E2" s="2"/>
@@ -1406,12 +1416,12 @@
     </row>
     <row r="3" ht="15" customHeight="1">
       <c r="A3" s="2"/>
-      <c r="B3" t="s" s="5">
+      <c r="B3" t="s" s="6">
         <v>4</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -1419,182 +1429,182 @@
       <c r="J3" s="2"/>
     </row>
     <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="7"/>
-      <c r="B4" t="s" s="8">
+      <c r="A4" s="8"/>
+      <c r="B4" t="s" s="9">
         <v>5</v>
       </c>
-      <c r="C4" t="s" s="8">
+      <c r="C4" t="s" s="9">
         <v>6</v>
       </c>
-      <c r="D4" t="s" s="8">
+      <c r="D4" t="s" s="9">
         <v>7</v>
       </c>
-      <c r="E4" t="s" s="8">
+      <c r="E4" t="s" s="9">
         <v>8</v>
       </c>
-      <c r="F4" s="9"/>
+      <c r="F4" s="10"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
     <row r="5" ht="41.75" customHeight="1">
-      <c r="A5" s="7"/>
-      <c r="B5" t="s" s="10">
+      <c r="A5" s="8"/>
+      <c r="B5" t="s" s="11">
         <v>9</v>
       </c>
-      <c r="C5" t="s" s="10">
+      <c r="C5" t="s" s="11">
         <v>10</v>
       </c>
-      <c r="D5" t="s" s="10">
+      <c r="D5" t="s" s="11">
         <v>11</v>
       </c>
-      <c r="E5" t="s" s="10">
+      <c r="E5" t="s" s="11">
         <v>12</v>
       </c>
-      <c r="F5" t="s" s="11">
+      <c r="F5" t="s" s="12">
         <v>13</v>
       </c>
-      <c r="G5" t="s" s="4">
+      <c r="G5" t="s" s="5">
         <v>14</v>
       </c>
-      <c r="H5" t="s" s="4">
+      <c r="H5" t="s" s="5">
         <v>15</v>
       </c>
-      <c r="I5" t="s" s="4">
+      <c r="I5" t="s" s="5">
         <v>16</v>
       </c>
-      <c r="J5" t="s" s="4">
+      <c r="J5" t="s" s="5">
         <v>17</v>
       </c>
     </row>
     <row r="6" ht="41.75" customHeight="1">
-      <c r="A6" s="7"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="9"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="10"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
     <row r="7" ht="41.75" customHeight="1">
-      <c r="A7" s="7"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="9"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="10"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
     <row r="8" ht="41.75" customHeight="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="9"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="10"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
     <row r="9" ht="41.75" customHeight="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="9"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="10"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
     <row r="10" ht="41.75" customHeight="1">
-      <c r="A10" s="7"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="9"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="10"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
     <row r="11" ht="41.75" customHeight="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="9"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="10"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
     <row r="12" ht="41.75" customHeight="1">
-      <c r="A12" s="7"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="9"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="10"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
     <row r="13" ht="41.75" customHeight="1">
-      <c r="A13" s="7"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="9"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="10"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" ht="41.75" customHeight="1">
-      <c r="A14" s="7"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="9"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="10"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" ht="41.75" customHeight="1">
-      <c r="A15" s="7"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="9"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="10"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" ht="41.75" customHeight="1">
-      <c r="A16" s="7"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="9"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="10"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -1618,8 +1628,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.8" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="10.2109" style="13" customWidth="1"/>
-    <col min="6" max="256" width="12" style="13" customWidth="1"/>
+    <col min="1" max="5" width="10.2109" style="14" customWidth="1"/>
+    <col min="6" max="256" width="12" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
@@ -1710,8 +1720,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.8" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="10.2109" style="14" customWidth="1"/>
-    <col min="6" max="256" width="12" style="14" customWidth="1"/>
+    <col min="1" max="5" width="10.2109" style="15" customWidth="1"/>
+    <col min="6" max="256" width="12" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">

</xml_diff>

<commit_message>
Support formula re-calc #21
(cherry picked from commit 6c9684ac4c2f9def4bd4efd978b677fdf0928a87)
</commit_message>
<xml_diff>
--- a/sample/report/template/sheet_02.xlsx
+++ b/sample/report/template/sheet_02.xlsx
@@ -104,7 +104,7 @@
       <name val="TakaoPGothic"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,6 +127,19 @@
         </stop>
         <stop position="1">
           <color rgb="ffffe6e5"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill type="linear" degree="270">
+        <stop position="0">
+          <color rgb="ffa2c3ff"/>
+        </stop>
+        <stop position="0.35">
+          <color rgb="ffbdd3ff"/>
+        </stop>
+        <stop position="1">
+          <color rgb="ffe5eeff"/>
         </stop>
       </gradientFill>
     </fill>
@@ -226,7 +239,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -237,6 +250,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -254,7 +270,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1380,14 +1396,17 @@
       <c r="B1" t="s" s="3">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="4">
+      <c r="C1" s="4">
+        <f>COUNTA(B5:B16)</f>
+        <v>1</v>
+      </c>
+      <c r="D1" s="5">
         <v>123</v>
       </c>
-      <c r="E1" s="4">
+      <c r="E1" s="5">
         <v>456</v>
       </c>
-      <c r="F1" s="4">
+      <c r="F1" s="5">
         <f>D1+E1</f>
         <v>579</v>
       </c>
@@ -1398,13 +1417,13 @@
     </row>
     <row r="2" ht="15" customHeight="1">
       <c r="A2" s="2"/>
-      <c r="B2" t="s" s="5">
+      <c r="B2" t="s" s="6">
         <v>1</v>
       </c>
-      <c r="C2" t="s" s="5">
+      <c r="C2" t="s" s="6">
         <v>2</v>
       </c>
-      <c r="D2" t="s" s="5">
+      <c r="D2" t="s" s="6">
         <v>3</v>
       </c>
       <c r="E2" s="2"/>
@@ -1416,12 +1435,12 @@
     </row>
     <row r="3" ht="15" customHeight="1">
       <c r="A3" s="2"/>
-      <c r="B3" t="s" s="6">
+      <c r="B3" t="s" s="7">
         <v>4</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -1429,182 +1448,182 @@
       <c r="J3" s="2"/>
     </row>
     <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="8"/>
-      <c r="B4" t="s" s="9">
+      <c r="A4" s="9"/>
+      <c r="B4" t="s" s="10">
         <v>5</v>
       </c>
-      <c r="C4" t="s" s="9">
+      <c r="C4" t="s" s="10">
         <v>6</v>
       </c>
-      <c r="D4" t="s" s="9">
+      <c r="D4" t="s" s="10">
         <v>7</v>
       </c>
-      <c r="E4" t="s" s="9">
+      <c r="E4" t="s" s="10">
         <v>8</v>
       </c>
-      <c r="F4" s="10"/>
+      <c r="F4" s="11"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
     <row r="5" ht="41.75" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" t="s" s="11">
+      <c r="A5" s="9"/>
+      <c r="B5" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="C5" t="s" s="11">
+      <c r="C5" t="s" s="12">
         <v>10</v>
       </c>
-      <c r="D5" t="s" s="11">
+      <c r="D5" t="s" s="12">
         <v>11</v>
       </c>
-      <c r="E5" t="s" s="11">
+      <c r="E5" t="s" s="12">
         <v>12</v>
       </c>
-      <c r="F5" t="s" s="12">
+      <c r="F5" t="s" s="13">
         <v>13</v>
       </c>
-      <c r="G5" t="s" s="5">
+      <c r="G5" t="s" s="6">
         <v>14</v>
       </c>
-      <c r="H5" t="s" s="5">
+      <c r="H5" t="s" s="6">
         <v>15</v>
       </c>
-      <c r="I5" t="s" s="5">
+      <c r="I5" t="s" s="6">
         <v>16</v>
       </c>
-      <c r="J5" t="s" s="5">
+      <c r="J5" t="s" s="6">
         <v>17</v>
       </c>
     </row>
     <row r="6" ht="41.75" customHeight="1">
-      <c r="A6" s="8"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="10"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="11"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
     <row r="7" ht="41.75" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="10"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="11"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
     <row r="8" ht="41.75" customHeight="1">
-      <c r="A8" s="8"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="10"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="11"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
     <row r="9" ht="41.75" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="10"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="11"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
     <row r="10" ht="41.75" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="10"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="11"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
     <row r="11" ht="41.75" customHeight="1">
-      <c r="A11" s="8"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="10"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="11"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
     <row r="12" ht="41.75" customHeight="1">
-      <c r="A12" s="8"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="10"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="11"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
     <row r="13" ht="41.75" customHeight="1">
-      <c r="A13" s="8"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="10"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="11"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" ht="41.75" customHeight="1">
-      <c r="A14" s="8"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="10"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="11"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" ht="41.75" customHeight="1">
-      <c r="A15" s="8"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="10"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="11"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" ht="41.75" customHeight="1">
-      <c r="A16" s="8"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="10"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="11"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -1628,8 +1647,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.8" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="10.2109" style="14" customWidth="1"/>
-    <col min="6" max="256" width="12" style="14" customWidth="1"/>
+    <col min="1" max="5" width="10.2109" style="15" customWidth="1"/>
+    <col min="6" max="256" width="12" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
@@ -1720,8 +1739,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.8" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="10.2109" style="15" customWidth="1"/>
-    <col min="6" max="256" width="12" style="15" customWidth="1"/>
+    <col min="1" max="5" width="10.2109" style="16" customWidth="1"/>
+    <col min="6" max="256" width="12" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">

</xml_diff>